<commit_message>
Modified the signup page
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/fb/keyword/scenarios/KeywordDriver.xlsx
+++ b/src/main/java/com/qa/fb/keyword/scenarios/KeywordDriver.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>Test step</t>
   </si>
@@ -59,9 +59,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>cssSelector</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>login</t>
   </si>
   <si>
-    <t>//span(text)-"Sinky Verma"</t>
-  </si>
-  <si>
     <t>quit</t>
   </si>
   <si>
@@ -92,12 +86,6 @@
     <t>sendKeys</t>
   </si>
   <si>
-    <t>Enter url</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/</t>
   </si>
   <si>
@@ -116,18 +104,6 @@
     <t>locatorValue</t>
   </si>
   <si>
-    <t>verify signup link</t>
-  </si>
-  <si>
-    <t>close browser</t>
-  </si>
-  <si>
-    <t>linktext</t>
-  </si>
-  <si>
-    <t>Sign up</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -137,13 +113,97 @@
     <t>Click</t>
   </si>
   <si>
-    <t>Quit</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>Click On Create new account Button</t>
+  </si>
+  <si>
+    <t>SurName</t>
+  </si>
+  <si>
+    <t>MobileNumber or Email Address</t>
+  </si>
+  <si>
+    <t>Re-Enter email address</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Select Gender radio button</t>
+  </si>
+  <si>
+    <t>Click on signUp button</t>
+  </si>
+  <si>
+    <t>sendkeys</t>
+  </si>
+  <si>
+    <t>Sinky</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Create New Account</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>//label[text()='Female']</t>
+  </si>
+  <si>
+    <t>websubmit</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>//input[@name='firstname']</t>
+  </si>
+  <si>
+    <t>//input[@name='lastname']</t>
+  </si>
+  <si>
+    <t>//input[@name='reg_email__']</t>
+  </si>
+  <si>
+    <t>//input[@name='reg_email_confirmation__']</t>
+  </si>
+  <si>
+    <t>//input[@name='reg_passwd__']</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Select date from drop down</t>
+  </si>
+  <si>
+    <t>Select month from drop down</t>
+  </si>
+  <si>
+    <t>select year from drop down</t>
   </si>
 </sst>
 </file>
@@ -490,15 +550,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
@@ -534,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -548,10 +608,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -559,16 +619,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -576,16 +636,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -593,13 +653,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -610,13 +670,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -633,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -650,36 +710,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -696,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -710,24 +770,24 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -735,24 +795,196 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>